<commit_message>
Add tests for escaping in urls
Tests are failing, but will hopefully be fixed in next commit
</commit_message>
<xml_diff>
--- a/IntoRdf.Tests/TestData/escaping.xlsx
+++ b/IntoRdf.Tests/TestData/escaping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\toftalisk\esrc\into-rdf\IntoRdf.Tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473027C5-FA5F-43C7-9348-BD1ABB0DB514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3678195C-EC72-4775-A61A-1277999732FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{C84AD5CC-CE77-43D9-8919-5BC7B90D77AF}"/>
   </bookViews>
@@ -50,9 +50,6 @@
     <t>backslash</t>
   </si>
   <si>
-    <t xml:space="preserve">space </t>
-  </si>
-  <si>
     <t>v/v</t>
   </si>
   <si>
@@ -103,6 +100,9 @@
   </si>
   <si>
     <t>v"""v</t>
+  </si>
+  <si>
+    <t>space</t>
   </si>
 </sst>
 </file>
@@ -460,7 +460,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,7 +481,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -489,71 +489,71 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
         <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
         <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
         <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add more test cases for escaping
</commit_message>
<xml_diff>
--- a/IntoRdf.Tests/TestData/escaping.xlsx
+++ b/IntoRdf.Tests/TestData/escaping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\toftalisk\esrc\into-rdf\IntoRdf.Tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3678195C-EC72-4775-A61A-1277999732FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92EA481-02E4-41DF-8833-BADC72E080FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{C84AD5CC-CE77-43D9-8919-5BC7B90D77AF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -103,6 +103,30 @@
   </si>
   <si>
     <t>space</t>
+  </si>
+  <si>
+    <t>dot</t>
+  </si>
+  <si>
+    <t>v.v</t>
+  </si>
+  <si>
+    <t>comma</t>
+  </si>
+  <si>
+    <t>v,v</t>
+  </si>
+  <si>
+    <t>trailing1</t>
+  </si>
+  <si>
+    <t>trailing2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vv2  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">vv1 </t>
   </si>
 </sst>
 </file>
@@ -457,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B654BC1F-5AC1-4924-A358-CAA1FE0DDC3A}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,6 +580,38 @@
         <v>20</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add pipe and colon
`|` and `:` broke into rdf, manually escape them
</commit_message>
<xml_diff>
--- a/IntoRdf.Tests/TestData/escaping.xlsx
+++ b/IntoRdf.Tests/TestData/escaping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\toftalisk\esrc\into-rdf\IntoRdf.Tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92EA481-02E4-41DF-8833-BADC72E080FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE3C38E-4A22-4FE1-903A-3178D3A2A9F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{C84AD5CC-CE77-43D9-8919-5BC7B90D77AF}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{C84AD5CC-CE77-43D9-8919-5BC7B90D77AF}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Name</t>
   </si>
@@ -127,16 +127,126 @@
   </si>
   <si>
     <t xml:space="preserve">vv1 </t>
+  </si>
+  <si>
+    <t>exclamation</t>
+  </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>v?v</t>
+  </si>
+  <si>
+    <t>v!v</t>
+  </si>
+  <si>
+    <t>doubleQuestion</t>
+  </si>
+  <si>
+    <t>v?v?v</t>
+  </si>
+  <si>
+    <t>v+v</t>
+  </si>
+  <si>
+    <t>v-v</t>
+  </si>
+  <si>
+    <t>plus</t>
+  </si>
+  <si>
+    <t>minus</t>
+  </si>
+  <si>
+    <t>star</t>
+  </si>
+  <si>
+    <t>v*v</t>
+  </si>
+  <si>
+    <t>hash</t>
+  </si>
+  <si>
+    <t>v#v</t>
+  </si>
+  <si>
+    <t>doubleHash</t>
+  </si>
+  <si>
+    <t>v#v#v</t>
+  </si>
+  <si>
+    <t>percent</t>
+  </si>
+  <si>
+    <t>v%v</t>
+  </si>
+  <si>
+    <t>ampersand</t>
+  </si>
+  <si>
+    <t>v&amp;v</t>
+  </si>
+  <si>
+    <t>equal</t>
+  </si>
+  <si>
+    <t>v=v</t>
+  </si>
+  <si>
+    <t>v@v</t>
+  </si>
+  <si>
+    <t>colon</t>
+  </si>
+  <si>
+    <t>v:v</t>
+  </si>
+  <si>
+    <t>at</t>
+  </si>
+  <si>
+    <t>gt</t>
+  </si>
+  <si>
+    <t>lt</t>
+  </si>
+  <si>
+    <t>pipe</t>
+  </si>
+  <si>
+    <t>semicolon</t>
+  </si>
+  <si>
+    <t>v&gt;v</t>
+  </si>
+  <si>
+    <t>v|v</t>
+  </si>
+  <si>
+    <t>v;v</t>
+  </si>
+  <si>
+    <t>v&lt;v</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -159,16 +269,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperkobling" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -481,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B654BC1F-5AC1-4924-A358-CAA1FE0DDC3A}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,7 +725,146 @@
         <v>28</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B27" r:id="rId1" xr:uid="{3582A621-093C-46DF-953E-95A35BA772D9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add escaping for urls (#11)
If special characters in for example an excel cell should genererate a uri we want:

```
/ -> %2f
\ -> %5c
# -> %23
: -> %3a
\ -> %7c
```

All other characters should be escaped as they are done be C#'s `System.Uri`.

Add comprehensive tests for the 4 special character and a lot of others + trailing whitespace tests
</commit_message>
<xml_diff>
--- a/IntoRdf.Tests/TestData/escaping.xlsx
+++ b/IntoRdf.Tests/TestData/escaping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\toftalisk\esrc\into-rdf\IntoRdf.Tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473027C5-FA5F-43C7-9348-BD1ABB0DB514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE3C38E-4A22-4FE1-903A-3178D3A2A9F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{C84AD5CC-CE77-43D9-8919-5BC7B90D77AF}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{C84AD5CC-CE77-43D9-8919-5BC7B90D77AF}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Name</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>backslash</t>
-  </si>
-  <si>
-    <t xml:space="preserve">space </t>
   </si>
   <si>
     <t>v/v</t>
@@ -103,16 +100,153 @@
   </si>
   <si>
     <t>v"""v</t>
+  </si>
+  <si>
+    <t>space</t>
+  </si>
+  <si>
+    <t>dot</t>
+  </si>
+  <si>
+    <t>v.v</t>
+  </si>
+  <si>
+    <t>comma</t>
+  </si>
+  <si>
+    <t>v,v</t>
+  </si>
+  <si>
+    <t>trailing1</t>
+  </si>
+  <si>
+    <t>trailing2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vv2  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">vv1 </t>
+  </si>
+  <si>
+    <t>exclamation</t>
+  </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>v?v</t>
+  </si>
+  <si>
+    <t>v!v</t>
+  </si>
+  <si>
+    <t>doubleQuestion</t>
+  </si>
+  <si>
+    <t>v?v?v</t>
+  </si>
+  <si>
+    <t>v+v</t>
+  </si>
+  <si>
+    <t>v-v</t>
+  </si>
+  <si>
+    <t>plus</t>
+  </si>
+  <si>
+    <t>minus</t>
+  </si>
+  <si>
+    <t>star</t>
+  </si>
+  <si>
+    <t>v*v</t>
+  </si>
+  <si>
+    <t>hash</t>
+  </si>
+  <si>
+    <t>v#v</t>
+  </si>
+  <si>
+    <t>doubleHash</t>
+  </si>
+  <si>
+    <t>v#v#v</t>
+  </si>
+  <si>
+    <t>percent</t>
+  </si>
+  <si>
+    <t>v%v</t>
+  </si>
+  <si>
+    <t>ampersand</t>
+  </si>
+  <si>
+    <t>v&amp;v</t>
+  </si>
+  <si>
+    <t>equal</t>
+  </si>
+  <si>
+    <t>v=v</t>
+  </si>
+  <si>
+    <t>v@v</t>
+  </si>
+  <si>
+    <t>colon</t>
+  </si>
+  <si>
+    <t>v:v</t>
+  </si>
+  <si>
+    <t>at</t>
+  </si>
+  <si>
+    <t>gt</t>
+  </si>
+  <si>
+    <t>lt</t>
+  </si>
+  <si>
+    <t>pipe</t>
+  </si>
+  <si>
+    <t>semicolon</t>
+  </si>
+  <si>
+    <t>v&gt;v</t>
+  </si>
+  <si>
+    <t>v|v</t>
+  </si>
+  <si>
+    <t>v;v</t>
+  </si>
+  <si>
+    <t>v&lt;v</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -135,16 +269,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperkobling" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -457,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B654BC1F-5AC1-4924-A358-CAA1FE0DDC3A}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,7 +618,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -489,74 +626,245 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
         <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
         <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
-        <v>21</v>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B27" r:id="rId1" xr:uid="{3582A621-093C-46DF-953E-95A35BA772D9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>